<commit_message>
fix: the remaining bugs and updated testGrid.xlsx
</commit_message>
<xml_diff>
--- a/packages/ui/cypress/TestGrid.xlsx
+++ b/packages/ui/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83C2B9-3766-48CA-AB22-42DC81B25750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA75BA5-E179-4D86-8D77-3239B14B4732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="553">
   <si>
     <t>Page</t>
   </si>
@@ -2164,6 +2164,9 @@
   </si>
   <si>
     <t>All tests that use the train.TypeYourMessage() function.</t>
+  </si>
+  <si>
+    <t>Type user turn - Verify that either no entities are detected, or the ones that are detected are expected. (Bug 2396)</t>
   </si>
 </sst>
 </file>
@@ -2468,86 +2471,95 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$27</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>43819</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43798</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2555,86 +2567,95 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$27</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>248</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>242</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>234</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>229</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>183</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>166</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -2671,86 +2692,95 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$27</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>43819</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43798</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2758,86 +2788,95 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$27</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -3609,13 +3648,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3647,8 +3686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F311" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F311" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F312" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F312" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3677,8 +3716,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D27" totalsRowShown="0">
-  <autoFilter ref="A1:D27" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -4081,11 +4120,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F291"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A291" sqref="A291:XFD291"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5243,16 +5282,16 @@
         <v>45</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>307</v>
+        <v>552</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>398</v>
+        <v>551</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5266,7 +5305,7 @@
         <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>398</v>
@@ -5283,7 +5322,7 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>398</v>
@@ -5300,7 +5339,7 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>398</v>
@@ -5317,7 +5356,7 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>398</v>
@@ -5334,7 +5373,7 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>398</v>
@@ -5351,13 +5390,13 @@
         <v>14</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>399</v>
+        <v>306</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -5368,7 +5407,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>403</v>
@@ -5385,13 +5424,13 @@
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>45</v>
       </c>
@@ -5402,7 +5441,7 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>403</v>
@@ -5419,13 +5458,13 @@
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>45</v>
       </c>
@@ -5436,13 +5475,13 @@
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -5453,13 +5492,13 @@
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -5470,13 +5509,13 @@
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>45</v>
       </c>
@@ -5487,13 +5526,13 @@
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>45</v>
       </c>
@@ -5504,10 +5543,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -5521,7 +5560,7 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>412</v>
@@ -5538,13 +5577,13 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -5555,13 +5594,13 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -5572,13 +5611,13 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -5589,10 +5628,10 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5606,13 +5645,13 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -5623,10 +5662,10 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>312</v>
+        <v>418</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>248</v>
+        <v>419</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -5640,10 +5679,10 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>465</v>
+        <v>312</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>476</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -5657,7 +5696,7 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>476</v>
@@ -5674,13 +5713,13 @@
         <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -5691,13 +5730,13 @@
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -5708,7 +5747,7 @@
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>476</v>
@@ -5725,7 +5764,7 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>476</v>
@@ -5742,7 +5781,7 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>476</v>
@@ -5759,13 +5798,13 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>45</v>
       </c>
@@ -5776,7 +5815,7 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>476</v>
@@ -5793,7 +5832,7 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>476</v>
@@ -5810,13 +5849,13 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -5827,10 +5866,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>533</v>
+        <v>475</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>542</v>
+        <v>476</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5838,19 +5877,19 @@
         <v>45</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>422</v>
+        <v>533</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>45</v>
       </c>
@@ -5861,13 +5900,13 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>45</v>
       </c>
@@ -5878,30 +5917,30 @@
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>45</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>45</v>
       </c>
@@ -5912,13 +5951,13 @@
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>45</v>
       </c>
@@ -5929,27 +5968,27 @@
         <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>45</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -5963,7 +6002,7 @@
         <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>231</v>
@@ -5980,7 +6019,7 @@
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>231</v>
@@ -5997,7 +6036,7 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>231</v>
@@ -6014,13 +6053,13 @@
         <v>14</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>45</v>
       </c>
@@ -6031,13 +6070,13 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>45</v>
       </c>
@@ -6048,10 +6087,10 @@
         <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>232</v>
+        <v>62</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -6065,13 +6104,13 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>435</v>
+        <v>232</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>45</v>
       </c>
@@ -6082,7 +6121,7 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>445</v>
@@ -6093,13 +6132,13 @@
         <v>45</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>445</v>
@@ -6116,13 +6155,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>45</v>
       </c>
@@ -6133,7 +6172,7 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>445</v>
@@ -6150,13 +6189,13 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>45</v>
       </c>
@@ -6167,13 +6206,13 @@
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>45</v>
       </c>
@@ -6184,13 +6223,13 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>45</v>
       </c>
@@ -6201,30 +6240,30 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>45</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -6235,30 +6274,30 @@
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>45</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>55</v>
+        <v>430</v>
       </c>
       <c r="C125" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>376</v>
+        <v>434</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>45</v>
       </c>
@@ -6269,13 +6308,13 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>45</v>
       </c>
@@ -6286,7 +6325,7 @@
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>458</v>
@@ -6303,13 +6342,13 @@
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>45</v>
       </c>
@@ -6320,13 +6359,13 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>45</v>
       </c>
@@ -6337,7 +6376,7 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>458</v>
@@ -6354,7 +6393,7 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>458</v>
@@ -6371,27 +6410,27 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>45</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="C133" t="s">
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6405,13 +6444,13 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>314</v>
+        <v>459</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>45</v>
       </c>
@@ -6422,13 +6461,13 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>45</v>
       </c>
@@ -6439,7 +6478,7 @@
         <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>460</v>
+        <v>313</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>461</v>
@@ -6456,24 +6495,24 @@
         <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>45</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>198</v>
+        <v>277</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>461</v>
@@ -6490,7 +6529,7 @@
         <v>14</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>461</v>
@@ -6507,7 +6546,7 @@
         <v>14</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>461</v>
@@ -6524,7 +6563,7 @@
         <v>14</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>461</v>
@@ -6535,19 +6574,19 @@
         <v>45</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>38</v>
+        <v>464</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>45</v>
       </c>
@@ -6558,7 +6597,7 @@
         <v>14</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>231</v>
@@ -6575,10 +6614,10 @@
         <v>14</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6592,13 +6631,13 @@
         <v>14</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>45</v>
       </c>
@@ -6609,13 +6648,13 @@
         <v>14</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>45</v>
       </c>
@@ -6626,13 +6665,13 @@
         <v>14</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>45</v>
       </c>
@@ -6643,7 +6682,7 @@
         <v>14</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>234</v>
@@ -6660,7 +6699,7 @@
         <v>14</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>234</v>
@@ -6677,10 +6716,10 @@
         <v>14</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -6694,13 +6733,13 @@
         <v>14</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>45</v>
       </c>
@@ -6711,7 +6750,7 @@
         <v>14</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>231</v>
@@ -6728,16 +6767,13 @@
         <v>14</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>45</v>
       </c>
@@ -6748,30 +6784,33 @@
         <v>14</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F154" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>45</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C155" t="s">
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>45</v>
       </c>
@@ -6782,13 +6821,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>245</v>
+        <v>63</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>45</v>
       </c>
@@ -6799,13 +6838,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>45</v>
       </c>
@@ -6816,10 +6855,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>526</v>
+        <v>226</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6833,13 +6872,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>514</v>
+        <v>287</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>45</v>
       </c>
@@ -6850,13 +6889,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>45</v>
       </c>
@@ -6867,7 +6906,7 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>526</v>
@@ -6884,13 +6923,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>45</v>
       </c>
@@ -6901,13 +6940,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>45</v>
       </c>
@@ -6918,13 +6957,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>515</v>
+        <v>490</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>45</v>
       </c>
@@ -6932,27 +6971,27 @@
         <v>61</v>
       </c>
       <c r="C165" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>45</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>521</v>
+        <v>61</v>
       </c>
       <c r="C166" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>526</v>
@@ -6969,7 +7008,7 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>526</v>
@@ -6985,45 +7024,45 @@
       <c r="C168" t="s">
         <v>14</v>
       </c>
-      <c r="D168" s="8" t="s">
-        <v>522</v>
+      <c r="D168" s="3" t="s">
+        <v>516</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="F168" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>45</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>61</v>
+        <v>521</v>
       </c>
       <c r="C169" t="s">
         <v>14</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>518</v>
+      <c r="D169" s="8" t="s">
+        <v>522</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>526</v>
       </c>
+      <c r="F169" s="3" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>45</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>519</v>
+        <v>61</v>
       </c>
       <c r="C170" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>526</v>
@@ -7034,16 +7073,16 @@
         <v>45</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>61</v>
+        <v>519</v>
       </c>
       <c r="C171" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>286</v>
+        <v>527</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>505</v>
+        <v>526</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7057,7 +7096,7 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>510</v>
+        <v>286</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>505</v>
@@ -7074,13 +7113,13 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>487</v>
+        <v>510</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>45</v>
       </c>
@@ -7091,7 +7130,7 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>505</v>
@@ -7108,13 +7147,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>45</v>
       </c>
@@ -7125,13 +7164,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>45</v>
       </c>
@@ -7142,10 +7181,10 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7159,13 +7198,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>45</v>
       </c>
@@ -7176,13 +7215,13 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>492</v>
+        <v>511</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>45</v>
       </c>
@@ -7193,13 +7232,13 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>45</v>
       </c>
@@ -7210,13 +7249,13 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>45</v>
       </c>
@@ -7227,7 +7266,7 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>506</v>
@@ -7244,13 +7283,13 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>45</v>
       </c>
@@ -7261,13 +7300,13 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>45</v>
       </c>
@@ -7278,13 +7317,13 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>45</v>
       </c>
@@ -7295,13 +7334,13 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>45</v>
       </c>
@@ -7312,13 +7351,13 @@
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>486</v>
+        <v>501</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>45</v>
       </c>
@@ -7329,16 +7368,13 @@
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="F188" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>45</v>
       </c>
@@ -7349,13 +7385,16 @@
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F189" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>45</v>
       </c>
@@ -7366,13 +7405,13 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>420</v>
+        <v>513</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>45</v>
       </c>
@@ -7383,10 +7422,10 @@
         <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7394,16 +7433,16 @@
         <v>45</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C192" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>68</v>
+        <v>438</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>261</v>
+        <v>440</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7417,7 +7456,7 @@
         <v>12</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>261</v>
@@ -7434,7 +7473,7 @@
         <v>12</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>261</v>
@@ -7448,10 +7487,10 @@
         <v>67</v>
       </c>
       <c r="C195" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>261</v>
@@ -7468,13 +7507,13 @@
         <v>14</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>45</v>
       </c>
@@ -7484,11 +7523,11 @@
       <c r="C197" t="s">
         <v>14</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>73</v>
+      <c r="D197" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7502,10 +7541,10 @@
         <v>14</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7519,7 +7558,7 @@
         <v>14</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>248</v>
@@ -7536,10 +7575,10 @@
         <v>14</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7553,10 +7592,10 @@
         <v>14</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7570,13 +7609,13 @@
         <v>14</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>45</v>
       </c>
@@ -7586,14 +7625,14 @@
       <c r="C203" t="s">
         <v>14</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>79</v>
+      <c r="D203" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>45</v>
       </c>
@@ -7604,13 +7643,13 @@
         <v>14</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>45</v>
       </c>
@@ -7621,16 +7660,13 @@
         <v>14</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>477</v>
+        <v>80</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F205" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>45</v>
       </c>
@@ -7641,11 +7677,14 @@
         <v>14</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>485</v>
       </c>
+      <c r="F206" s="3" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
@@ -7658,7 +7697,7 @@
         <v>14</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>485</v>
@@ -7675,7 +7714,7 @@
         <v>14</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>485</v>
@@ -7692,13 +7731,13 @@
         <v>14</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>45</v>
       </c>
@@ -7709,13 +7748,13 @@
         <v>14</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>45</v>
       </c>
@@ -7726,44 +7765,41 @@
         <v>14</v>
       </c>
       <c r="D211" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>45</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C212" t="s">
+        <v>14</v>
+      </c>
+      <c r="D212" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>45</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C212" t="s">
-        <v>14</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F212" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>45</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>67</v>
+        <v>298</v>
       </c>
       <c r="C213" t="s">
         <v>14</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>528</v>
+        <v>299</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>281</v>
@@ -7772,7 +7808,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>45</v>
       </c>
@@ -7783,7 +7819,7 @@
         <v>14</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>281</v>
@@ -7792,7 +7828,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>45</v>
       </c>
@@ -7803,7 +7839,7 @@
         <v>14</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>281</v>
@@ -7812,7 +7848,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>45</v>
       </c>
@@ -7823,30 +7859,33 @@
         <v>14</v>
       </c>
       <c r="D216" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>45</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C217" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="E216" s="3" t="s">
+      <c r="E217" s="3" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>45</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C217" t="s">
-        <v>14</v>
-      </c>
-      <c r="D217" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E217" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>45</v>
       </c>
@@ -7857,13 +7896,13 @@
         <v>14</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>251</v>
+        <v>83</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>45</v>
       </c>
@@ -7874,13 +7913,13 @@
         <v>14</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>82</v>
+        <v>251</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>45</v>
       </c>
@@ -7891,7 +7930,7 @@
         <v>14</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>233</v>
@@ -7908,13 +7947,13 @@
         <v>14</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>536</v>
+        <v>84</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>45</v>
       </c>
@@ -7925,13 +7964,13 @@
         <v>14</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>91</v>
+        <v>536</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -7942,13 +7981,13 @@
         <v>14</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>45</v>
       </c>
@@ -7959,13 +7998,13 @@
         <v>14</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>45</v>
       </c>
@@ -7976,10 +8015,10 @@
         <v>14</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7993,10 +8032,10 @@
         <v>14</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>266</v>
+        <v>85</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8010,13 +8049,13 @@
         <v>14</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>95</v>
+        <v>266</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>45</v>
       </c>
@@ -8027,16 +8066,13 @@
         <v>14</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>319</v>
+        <v>95</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="F228" s="3" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>45</v>
       </c>
@@ -8047,27 +8083,30 @@
         <v>14</v>
       </c>
       <c r="D229" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>45</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C230" t="s">
+        <v>14</v>
+      </c>
+      <c r="D230" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E229" s="3" t="s">
+      <c r="E230" s="3" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>45</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="C230" t="s">
-        <v>14</v>
-      </c>
-      <c r="D230" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8075,19 +8114,19 @@
         <v>45</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C231" t="s">
         <v>14</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>45</v>
       </c>
@@ -8098,30 +8137,30 @@
         <v>14</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>15</v>
+        <v>540</v>
       </c>
       <c r="C233" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>89</v>
+        <v>541</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>15</v>
       </c>
@@ -8132,13 +8171,13 @@
         <v>15</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>15</v>
       </c>
@@ -8149,7 +8188,7 @@
         <v>15</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>390</v>
+        <v>88</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>388</v>
@@ -8160,19 +8199,19 @@
         <v>15</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>383</v>
+        <v>15</v>
       </c>
       <c r="C236" t="s">
         <v>15</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>15</v>
       </c>
@@ -8183,13 +8222,13 @@
         <v>15</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>15</v>
       </c>
@@ -8200,10 +8239,10 @@
         <v>15</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>253</v>
+        <v>384</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8217,10 +8256,10 @@
         <v>15</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>549</v>
+        <v>253</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8228,19 +8267,19 @@
         <v>15</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>15</v>
+        <v>383</v>
       </c>
       <c r="C240" t="s">
         <v>15</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>15</v>
       </c>
@@ -8251,13 +8290,13 @@
         <v>15</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>302</v>
+        <v>548</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>15</v>
       </c>
@@ -8268,30 +8307,30 @@
         <v>15</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>382</v>
+        <v>302</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="F242" s="3" t="s">
+    </row>
+    <row r="243" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>15</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C243" t="s">
+        <v>15</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F243" s="3" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>3</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C243" t="s">
-        <v>8</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8299,16 +8338,16 @@
         <v>3</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C244" t="s">
         <v>8</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>256</v>
+        <v>22</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
     </row>
     <row r="245" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8316,33 +8355,33 @@
         <v>3</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C245" t="s">
         <v>8</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>3</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -8350,13 +8389,13 @@
         <v>3</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="C247" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>281</v>
@@ -8370,7 +8409,7 @@
         <v>4</v>
       </c>
       <c r="C248" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>23</v>
@@ -8384,13 +8423,13 @@
         <v>3</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C249" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E249" s="3" t="s">
         <v>281</v>
@@ -8404,7 +8443,7 @@
         <v>5</v>
       </c>
       <c r="C250" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>24</v>
@@ -8413,18 +8452,18 @@
         <v>281</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>3</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C251" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>285</v>
+        <v>24</v>
       </c>
       <c r="E251" s="3" t="s">
         <v>281</v>
@@ -8432,16 +8471,16 @@
     </row>
     <row r="252" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
       <c r="C252" t="s">
-        <v>14</v>
+        <v>284</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="E252" s="3" t="s">
         <v>281</v>
@@ -8449,16 +8488,16 @@
     </row>
     <row r="253" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C253" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E253" s="3" t="s">
         <v>281</v>
@@ -8475,41 +8514,41 @@
         <v>269</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E254" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C255" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E255" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C256" t="s">
-        <v>14</v>
+        <v>275</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E256" s="3" t="s">
         <v>281</v>
@@ -8520,19 +8559,16 @@
         <v>45</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="C257" t="s">
         <v>14</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F257" s="3" t="s">
-        <v>320</v>
+        <v>281</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8546,11 +8582,14 @@
         <v>14</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E258" s="3" t="s">
         <v>350</v>
       </c>
+      <c r="F258" s="3" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="259" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -8563,7 +8602,7 @@
         <v>14</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E259" s="3" t="s">
         <v>350</v>
@@ -8580,7 +8619,7 @@
         <v>14</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="E260" s="3" t="s">
         <v>350</v>
@@ -8597,7 +8636,7 @@
         <v>14</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="E261" s="3" t="s">
         <v>350</v>
@@ -8614,7 +8653,7 @@
         <v>14</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="E262" s="3" t="s">
         <v>350</v>
@@ -8631,7 +8670,7 @@
         <v>14</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="E263" s="3" t="s">
         <v>350</v>
@@ -8648,7 +8687,7 @@
         <v>14</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="E264" s="3" t="s">
         <v>350</v>
@@ -8665,7 +8704,7 @@
         <v>14</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="E265" s="3" t="s">
         <v>350</v>
@@ -8682,7 +8721,7 @@
         <v>14</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E266" s="3" t="s">
         <v>350</v>
@@ -8699,13 +8738,13 @@
         <v>14</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="E267" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>45</v>
       </c>
@@ -8716,13 +8755,13 @@
         <v>14</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E268" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>45</v>
       </c>
@@ -8733,13 +8772,10 @@
         <v>14</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>290</v>
+        <v>356</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8753,7 +8789,7 @@
         <v>14</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E270" s="3" t="s">
         <v>340</v>
@@ -8773,10 +8809,10 @@
         <v>14</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E271" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F271" s="3" t="s">
         <v>318</v>
@@ -8793,7 +8829,7 @@
         <v>14</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E272" s="3" t="s">
         <v>341</v>
@@ -8813,10 +8849,10 @@
         <v>14</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="E273" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="F273" s="3" t="s">
         <v>318</v>
@@ -8833,7 +8869,7 @@
         <v>14</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E274" s="3" t="s">
         <v>348</v>
@@ -8842,7 +8878,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>45</v>
       </c>
@@ -8853,10 +8889,10 @@
         <v>14</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E275" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F275" s="3" t="s">
         <v>318</v>
@@ -8873,7 +8909,7 @@
         <v>14</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E276" s="3" t="s">
         <v>349</v>
@@ -8893,7 +8929,7 @@
         <v>14</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E277" s="3" t="s">
         <v>349</v>
@@ -8913,7 +8949,7 @@
         <v>14</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E278" s="3" t="s">
         <v>349</v>
@@ -8922,21 +8958,24 @@
         <v>318</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>45</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C279" t="s">
         <v>14</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="E279" s="3" t="s">
-        <v>361</v>
+        <v>349</v>
+      </c>
+      <c r="F279" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8950,7 +8989,7 @@
         <v>14</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E280" s="3" t="s">
         <v>361</v>
@@ -8967,7 +9006,7 @@
         <v>14</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E281" s="3" t="s">
         <v>361</v>
@@ -8984,7 +9023,7 @@
         <v>14</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E282" s="3" t="s">
         <v>361</v>
@@ -9001,13 +9040,13 @@
         <v>14</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>305</v>
+        <v>360</v>
       </c>
       <c r="E283" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>45</v>
       </c>
@@ -9018,14 +9057,11 @@
         <v>14</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="E284" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="F284" s="3" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="285" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
@@ -9038,7 +9074,7 @@
         <v>14</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E285" s="3" t="s">
         <v>330</v>
@@ -9047,7 +9083,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>45</v>
       </c>
@@ -9058,7 +9094,7 @@
         <v>14</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E286" s="3" t="s">
         <v>330</v>
@@ -9078,7 +9114,7 @@
         <v>14</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E287" s="3" t="s">
         <v>330</v>
@@ -9098,7 +9134,7 @@
         <v>14</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E288" s="3" t="s">
         <v>330</v>
@@ -9112,43 +9148,63 @@
         <v>45</v>
       </c>
       <c r="B289" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C289" t="s">
+        <v>14</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F289" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>45</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C289" t="s">
-        <v>14</v>
-      </c>
-      <c r="D289" s="3" t="s">
+      <c r="C290" t="s">
+        <v>14</v>
+      </c>
+      <c r="D290" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E289" s="3" t="s">
+      <c r="E290" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F289" s="3" t="s">
+      <c r="F290" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>45</v>
-      </c>
-      <c r="B290" s="3" t="s">
+    <row r="291" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>45</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C290" t="s">
-        <v>14</v>
-      </c>
-      <c r="D290" s="3" t="s">
+      <c r="C291" t="s">
+        <v>14</v>
+      </c>
+      <c r="D291" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E290" s="3" t="s">
+      <c r="E291" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="F290" s="3" t="s">
+      <c r="F291" s="3" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D291" s="15"/>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D292" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -9709,10 +9765,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9739,224 +9795,224 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43791</v>
+        <v>43819</v>
       </c>
       <c r="B2">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C24" si="0">SUM(B2,-D2)</f>
-        <v>254</v>
+        <f t="shared" ref="C2:C27" si="0">SUM(B2,-D2)</f>
+        <v>255</v>
       </c>
       <c r="D2">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43784</v>
+        <v>43812</v>
       </c>
       <c r="B3">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43777</v>
+        <v>43798</v>
       </c>
       <c r="B4">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D4">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43770</v>
+        <v>43791</v>
       </c>
       <c r="B5">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D5">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>43763</v>
+        <v>43784</v>
       </c>
       <c r="B6">
         <v>284</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>43756</v>
+        <v>43777</v>
       </c>
       <c r="B7">
         <v>284</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D7">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>43749</v>
+        <v>43770</v>
       </c>
       <c r="B8">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D8">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>43742</v>
+        <v>43763</v>
       </c>
       <c r="B9">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="D9">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>43735</v>
+        <v>43756</v>
       </c>
       <c r="B10">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>43728</v>
+        <v>43749</v>
       </c>
       <c r="B11">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="D11">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>43721</v>
+        <v>43742</v>
       </c>
       <c r="B12">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D12">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>43714</v>
+        <v>43735</v>
       </c>
       <c r="B13">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="D13">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>43707</v>
+        <v>43728</v>
       </c>
       <c r="B14">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="D14">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>43700</v>
+        <v>43721</v>
       </c>
       <c r="B15">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="D15">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>43693</v>
+        <v>43714</v>
       </c>
       <c r="B16">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="D16">
         <v>41</v>
@@ -9964,166 +10020,211 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>43665</v>
+        <v>43707</v>
       </c>
       <c r="B17">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="D17">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <v>43658</v>
+        <v>43700</v>
       </c>
       <c r="B18">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="D18">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>43651</v>
+        <v>43693</v>
       </c>
       <c r="B19">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="D19">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>43644</v>
+        <v>43665</v>
       </c>
       <c r="B20">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D20">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>43638</v>
+        <v>43658</v>
       </c>
       <c r="B21">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="D21">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>43630</v>
+        <v>43651</v>
       </c>
       <c r="B22">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D22">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>43623</v>
+        <v>43644</v>
       </c>
       <c r="B23">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D23">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>43616</v>
+        <v>43638</v>
       </c>
       <c r="B24">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="D24">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>43609</v>
+        <v>43630</v>
       </c>
       <c r="B25">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C25">
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>110</v>
       </c>
       <c r="D25">
-        <f>B25-C25</f>
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>43602</v>
+        <v>43623</v>
       </c>
       <c r="B26">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C26">
-        <v>79</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="D26">
-        <f>B26-C26</f>
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
+        <v>43616</v>
+      </c>
+      <c r="B27">
+        <v>186</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="D27">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>43609</v>
+      </c>
+      <c r="B28">
+        <v>185</v>
+      </c>
+      <c r="C28">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <f>B28-C28</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>43602</v>
+      </c>
+      <c r="B29">
+        <v>183</v>
+      </c>
+      <c r="C29">
+        <v>79</v>
+      </c>
+      <c r="D29">
+        <f>B29-C29</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
         <v>43595</v>
       </c>
-      <c r="B27">
+      <c r="B30">
         <v>172</v>
       </c>
-      <c r="C27">
+      <c r="C30">
         <v>76</v>
       </c>
-      <c r="D27">
-        <f>B27-C27</f>
+      <c r="D30">
+        <f>B30-C30</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Verify entity detection (#21)
Everytime the user types in a Train Dialog chat message it verifies that automatic entity detection is as expected.
</commit_message>
<xml_diff>
--- a/packages/ui/cypress/TestGrid.xlsx
+++ b/packages/ui/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D83C2B9-3766-48CA-AB22-42DC81B25750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA75BA5-E179-4D86-8D77-3239B14B4732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="553">
   <si>
     <t>Page</t>
   </si>
@@ -2164,6 +2164,9 @@
   </si>
   <si>
     <t>All tests that use the train.TypeYourMessage() function.</t>
+  </si>
+  <si>
+    <t>Type user turn - Verify that either no entities are detected, or the ones that are detected are expected. (Bug 2396)</t>
   </si>
 </sst>
 </file>
@@ -2468,86 +2471,95 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$27</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>43819</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43798</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2555,86 +2567,95 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$27</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>248</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>246</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>242</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>234</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>229</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>183</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>166</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -2671,86 +2692,95 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$27</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>43819</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43798</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2758,86 +2788,95 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$27</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="27">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -3609,13 +3648,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3647,8 +3686,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F311" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F311" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F312" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F312" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -3677,8 +3716,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D27" totalsRowShown="0">
-  <autoFilter ref="A1:D27" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D30" totalsRowShown="0">
+  <autoFilter ref="A1:D30" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -4081,11 +4120,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F291"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A291" sqref="A291:XFD291"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5243,16 +5282,16 @@
         <v>45</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>307</v>
+        <v>552</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>398</v>
+        <v>551</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5266,7 +5305,7 @@
         <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>398</v>
@@ -5283,7 +5322,7 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>398</v>
@@ -5300,7 +5339,7 @@
         <v>14</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>398</v>
@@ -5317,7 +5356,7 @@
         <v>14</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>398</v>
@@ -5334,7 +5373,7 @@
         <v>14</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>398</v>
@@ -5351,13 +5390,13 @@
         <v>14</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>399</v>
+        <v>306</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -5368,7 +5407,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>403</v>
@@ -5385,13 +5424,13 @@
         <v>14</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>45</v>
       </c>
@@ -5402,7 +5441,7 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>403</v>
@@ -5419,13 +5458,13 @@
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>45</v>
       </c>
@@ -5436,13 +5475,13 @@
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -5453,13 +5492,13 @@
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>45</v>
       </c>
@@ -5470,13 +5509,13 @@
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>45</v>
       </c>
@@ -5487,13 +5526,13 @@
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E80" s="3" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>45</v>
       </c>
@@ -5504,10 +5543,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -5521,7 +5560,7 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E82" s="3" t="s">
         <v>412</v>
@@ -5538,13 +5577,13 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>45</v>
       </c>
@@ -5555,13 +5594,13 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>45</v>
       </c>
@@ -5572,13 +5611,13 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -5589,10 +5628,10 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5606,13 +5645,13 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -5623,10 +5662,10 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>312</v>
+        <v>418</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>248</v>
+        <v>419</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -5640,10 +5679,10 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>465</v>
+        <v>312</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>476</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -5657,7 +5696,7 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>476</v>
@@ -5674,13 +5713,13 @@
         <v>14</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>45</v>
       </c>
@@ -5691,13 +5730,13 @@
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -5708,7 +5747,7 @@
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>476</v>
@@ -5725,7 +5764,7 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>476</v>
@@ -5742,7 +5781,7 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>476</v>
@@ -5759,13 +5798,13 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>45</v>
       </c>
@@ -5776,7 +5815,7 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>476</v>
@@ -5793,7 +5832,7 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E98" s="3" t="s">
         <v>476</v>
@@ -5810,13 +5849,13 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>45</v>
       </c>
@@ -5827,10 +5866,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>533</v>
+        <v>475</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>542</v>
+        <v>476</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5838,19 +5877,19 @@
         <v>45</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>422</v>
+        <v>533</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>45</v>
       </c>
@@ -5861,13 +5900,13 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>45</v>
       </c>
@@ -5878,30 +5917,30 @@
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>45</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C104" t="s">
         <v>14</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>45</v>
       </c>
@@ -5912,13 +5951,13 @@
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>45</v>
       </c>
@@ -5929,27 +5968,27 @@
         <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>45</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>442</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>45</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -5963,7 +6002,7 @@
         <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>231</v>
@@ -5980,7 +6019,7 @@
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>231</v>
@@ -5997,7 +6036,7 @@
         <v>14</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>231</v>
@@ -6014,13 +6053,13 @@
         <v>14</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>45</v>
       </c>
@@ -6031,13 +6070,13 @@
         <v>14</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>45</v>
       </c>
@@ -6048,10 +6087,10 @@
         <v>14</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>232</v>
+        <v>62</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -6065,13 +6104,13 @@
         <v>14</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>435</v>
+        <v>232</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>45</v>
       </c>
@@ -6082,7 +6121,7 @@
         <v>14</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>445</v>
@@ -6093,13 +6132,13 @@
         <v>45</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>445</v>
@@ -6116,13 +6155,13 @@
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>431</v>
+        <v>444</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>45</v>
       </c>
@@ -6133,7 +6172,7 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>445</v>
@@ -6150,13 +6189,13 @@
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="120" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>45</v>
       </c>
@@ -6167,13 +6206,13 @@
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>45</v>
       </c>
@@ -6184,13 +6223,13 @@
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>45</v>
       </c>
@@ -6201,30 +6240,30 @@
         <v>14</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>45</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>45</v>
       </c>
@@ -6235,30 +6274,30 @@
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>45</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>55</v>
+        <v>430</v>
       </c>
       <c r="C125" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>376</v>
+        <v>434</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>45</v>
       </c>
@@ -6269,13 +6308,13 @@
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>455</v>
+        <v>376</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>45</v>
       </c>
@@ -6286,7 +6325,7 @@
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>458</v>
@@ -6303,13 +6342,13 @@
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>45</v>
       </c>
@@ -6320,13 +6359,13 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>45</v>
       </c>
@@ -6337,7 +6376,7 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>458</v>
@@ -6354,7 +6393,7 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>458</v>
@@ -6371,27 +6410,27 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E132" s="3" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>45</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>277</v>
+        <v>55</v>
       </c>
       <c r="C133" t="s">
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6405,13 +6444,13 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>314</v>
+        <v>459</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>45</v>
       </c>
@@ -6422,13 +6461,13 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>45</v>
       </c>
@@ -6439,7 +6478,7 @@
         <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>460</v>
+        <v>313</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>461</v>
@@ -6456,24 +6495,24 @@
         <v>14</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>45</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>198</v>
+        <v>277</v>
       </c>
       <c r="C138" t="s">
         <v>14</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>461</v>
@@ -6490,7 +6529,7 @@
         <v>14</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>461</v>
@@ -6507,7 +6546,7 @@
         <v>14</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>461</v>
@@ -6524,7 +6563,7 @@
         <v>14</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>461</v>
@@ -6535,19 +6574,19 @@
         <v>45</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>38</v>
+        <v>464</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>45</v>
       </c>
@@ -6558,7 +6597,7 @@
         <v>14</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>231</v>
@@ -6575,10 +6614,10 @@
         <v>14</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6592,13 +6631,13 @@
         <v>14</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E145" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>45</v>
       </c>
@@ -6609,13 +6648,13 @@
         <v>14</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="E146" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>45</v>
       </c>
@@ -6626,13 +6665,13 @@
         <v>14</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E147" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>45</v>
       </c>
@@ -6643,7 +6682,7 @@
         <v>14</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E148" s="3" t="s">
         <v>234</v>
@@ -6660,7 +6699,7 @@
         <v>14</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>234</v>
@@ -6677,10 +6716,10 @@
         <v>14</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -6694,13 +6733,13 @@
         <v>14</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E151" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>45</v>
       </c>
@@ -6711,7 +6750,7 @@
         <v>14</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>231</v>
@@ -6728,16 +6767,13 @@
         <v>14</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>45</v>
       </c>
@@ -6748,30 +6784,33 @@
         <v>14</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E154" s="3" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F154" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>45</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C155" t="s">
         <v>14</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>45</v>
       </c>
@@ -6782,13 +6821,13 @@
         <v>14</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>245</v>
+        <v>63</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>45</v>
       </c>
@@ -6799,13 +6838,13 @@
         <v>14</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>45</v>
       </c>
@@ -6816,10 +6855,10 @@
         <v>14</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>526</v>
+        <v>226</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6833,13 +6872,13 @@
         <v>14</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>514</v>
+        <v>287</v>
       </c>
       <c r="E159" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>45</v>
       </c>
@@ -6850,13 +6889,13 @@
         <v>14</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>489</v>
+        <v>514</v>
       </c>
       <c r="E160" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>45</v>
       </c>
@@ -6867,7 +6906,7 @@
         <v>14</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E161" s="3" t="s">
         <v>526</v>
@@ -6884,13 +6923,13 @@
         <v>14</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>45</v>
       </c>
@@ -6901,13 +6940,13 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="E163" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>45</v>
       </c>
@@ -6918,13 +6957,13 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>515</v>
+        <v>490</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>45</v>
       </c>
@@ -6932,27 +6971,27 @@
         <v>61</v>
       </c>
       <c r="C165" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E165" s="3" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>45</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>521</v>
+        <v>61</v>
       </c>
       <c r="C166" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="E166" s="3" t="s">
         <v>526</v>
@@ -6969,7 +7008,7 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E167" s="3" t="s">
         <v>526</v>
@@ -6985,45 +7024,45 @@
       <c r="C168" t="s">
         <v>14</v>
       </c>
-      <c r="D168" s="8" t="s">
-        <v>522</v>
+      <c r="D168" s="3" t="s">
+        <v>516</v>
       </c>
       <c r="E168" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="F168" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>45</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>61</v>
+        <v>521</v>
       </c>
       <c r="C169" t="s">
         <v>14</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>518</v>
+      <c r="D169" s="8" t="s">
+        <v>522</v>
       </c>
       <c r="E169" s="3" t="s">
         <v>526</v>
       </c>
+      <c r="F169" s="3" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="170" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>45</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>519</v>
+        <v>61</v>
       </c>
       <c r="C170" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>526</v>
@@ -7034,16 +7073,16 @@
         <v>45</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>61</v>
+        <v>519</v>
       </c>
       <c r="C171" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>286</v>
+        <v>527</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>505</v>
+        <v>526</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7057,7 +7096,7 @@
         <v>14</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>510</v>
+        <v>286</v>
       </c>
       <c r="E172" s="3" t="s">
         <v>505</v>
@@ -7074,13 +7113,13 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>487</v>
+        <v>510</v>
       </c>
       <c r="E173" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="174" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>45</v>
       </c>
@@ -7091,7 +7130,7 @@
         <v>14</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
       <c r="E174" s="3" t="s">
         <v>505</v>
@@ -7108,13 +7147,13 @@
         <v>14</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="176" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>45</v>
       </c>
@@ -7125,13 +7164,13 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>45</v>
       </c>
@@ -7142,10 +7181,10 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7159,13 +7198,13 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>511</v>
+        <v>491</v>
       </c>
       <c r="E178" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>45</v>
       </c>
@@ -7176,13 +7215,13 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>492</v>
+        <v>511</v>
       </c>
       <c r="E179" s="3" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>45</v>
       </c>
@@ -7193,13 +7232,13 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>45</v>
       </c>
@@ -7210,13 +7249,13 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>498</v>
+        <v>508</v>
       </c>
       <c r="E181" s="3" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>45</v>
       </c>
@@ -7227,7 +7266,7 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>506</v>
@@ -7244,13 +7283,13 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>45</v>
       </c>
@@ -7261,13 +7300,13 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E184" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>45</v>
       </c>
@@ -7278,13 +7317,13 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="186" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>45</v>
       </c>
@@ -7295,13 +7334,13 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>45</v>
       </c>
@@ -7312,13 +7351,13 @@
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>486</v>
+        <v>501</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>45</v>
       </c>
@@ -7329,16 +7368,13 @@
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="F188" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>45</v>
       </c>
@@ -7349,13 +7385,16 @@
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="E189" s="3" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F189" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>45</v>
       </c>
@@ -7366,13 +7405,13 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>420</v>
+        <v>513</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>45</v>
       </c>
@@ -7383,10 +7422,10 @@
         <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7394,16 +7433,16 @@
         <v>45</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C192" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>68</v>
+        <v>438</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>261</v>
+        <v>440</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7417,7 +7456,7 @@
         <v>12</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E193" s="3" t="s">
         <v>261</v>
@@ -7434,7 +7473,7 @@
         <v>12</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E194" s="3" t="s">
         <v>261</v>
@@ -7448,10 +7487,10 @@
         <v>67</v>
       </c>
       <c r="C195" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E195" s="3" t="s">
         <v>261</v>
@@ -7468,13 +7507,13 @@
         <v>14</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E196" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>45</v>
       </c>
@@ -7484,11 +7523,11 @@
       <c r="C197" t="s">
         <v>14</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>73</v>
+      <c r="D197" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7502,10 +7541,10 @@
         <v>14</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E198" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7519,7 +7558,7 @@
         <v>14</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>248</v>
@@ -7536,10 +7575,10 @@
         <v>14</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7553,10 +7592,10 @@
         <v>14</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E201" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7570,13 +7609,13 @@
         <v>14</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>45</v>
       </c>
@@ -7586,14 +7625,14 @@
       <c r="C203" t="s">
         <v>14</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>79</v>
+      <c r="D203" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="204" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>45</v>
       </c>
@@ -7604,13 +7643,13 @@
         <v>14</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>45</v>
       </c>
@@ -7621,16 +7660,13 @@
         <v>14</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>477</v>
+        <v>80</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F205" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>45</v>
       </c>
@@ -7641,11 +7677,14 @@
         <v>14</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>485</v>
       </c>
+      <c r="F206" s="3" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
@@ -7658,7 +7697,7 @@
         <v>14</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E207" s="3" t="s">
         <v>485</v>
@@ -7675,7 +7714,7 @@
         <v>14</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="E208" s="3" t="s">
         <v>485</v>
@@ -7692,13 +7731,13 @@
         <v>14</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E209" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>45</v>
       </c>
@@ -7709,13 +7748,13 @@
         <v>14</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E210" s="3" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>45</v>
       </c>
@@ -7726,44 +7765,41 @@
         <v>14</v>
       </c>
       <c r="D211" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>45</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C212" t="s">
+        <v>14</v>
+      </c>
+      <c r="D212" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>45</v>
-      </c>
-      <c r="B212" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="C212" t="s">
-        <v>14</v>
-      </c>
-      <c r="D212" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="E212" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F212" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>45</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>67</v>
+        <v>298</v>
       </c>
       <c r="C213" t="s">
         <v>14</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>528</v>
+        <v>299</v>
       </c>
       <c r="E213" s="3" t="s">
         <v>281</v>
@@ -7772,7 +7808,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="214" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>45</v>
       </c>
@@ -7783,7 +7819,7 @@
         <v>14</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E214" s="3" t="s">
         <v>281</v>
@@ -7792,7 +7828,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="215" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>45</v>
       </c>
@@ -7803,7 +7839,7 @@
         <v>14</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>281</v>
@@ -7812,7 +7848,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="216" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>45</v>
       </c>
@@ -7823,30 +7859,33 @@
         <v>14</v>
       </c>
       <c r="D216" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>45</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C217" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="E216" s="3" t="s">
+      <c r="E217" s="3" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="217" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>45</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C217" t="s">
-        <v>14</v>
-      </c>
-      <c r="D217" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E217" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>45</v>
       </c>
@@ -7857,13 +7896,13 @@
         <v>14</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>251</v>
+        <v>83</v>
       </c>
       <c r="E218" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>45</v>
       </c>
@@ -7874,13 +7913,13 @@
         <v>14</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>82</v>
+        <v>251</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>45</v>
       </c>
@@ -7891,7 +7930,7 @@
         <v>14</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E220" s="3" t="s">
         <v>233</v>
@@ -7908,13 +7947,13 @@
         <v>14</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>536</v>
+        <v>84</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>45</v>
       </c>
@@ -7925,13 +7964,13 @@
         <v>14</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>91</v>
+        <v>536</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -7942,13 +7981,13 @@
         <v>14</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E223" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="224" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>45</v>
       </c>
@@ -7959,13 +7998,13 @@
         <v>14</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E224" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>45</v>
       </c>
@@ -7976,10 +8015,10 @@
         <v>14</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E225" s="3" t="s">
-        <v>233</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7993,10 +8032,10 @@
         <v>14</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>266</v>
+        <v>85</v>
       </c>
       <c r="E226" s="3" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
     </row>
     <row r="227" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8010,13 +8049,13 @@
         <v>14</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>95</v>
+        <v>266</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="228" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>45</v>
       </c>
@@ -8027,16 +8066,13 @@
         <v>14</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>319</v>
+        <v>95</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="F228" s="3" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>45</v>
       </c>
@@ -8047,27 +8083,30 @@
         <v>14</v>
       </c>
       <c r="D229" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>45</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C230" t="s">
+        <v>14</v>
+      </c>
+      <c r="D230" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E229" s="3" t="s">
+      <c r="E230" s="3" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>45</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="C230" t="s">
-        <v>14</v>
-      </c>
-      <c r="D230" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="E230" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8075,19 +8114,19 @@
         <v>45</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="C231" t="s">
         <v>14</v>
       </c>
       <c r="D231" s="3" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="E231" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="232" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>45</v>
       </c>
@@ -8098,30 +8137,30 @@
         <v>14</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="233" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>15</v>
+        <v>540</v>
       </c>
       <c r="C233" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>89</v>
+        <v>541</v>
       </c>
       <c r="E233" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>15</v>
       </c>
@@ -8132,13 +8171,13 @@
         <v>15</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>15</v>
       </c>
@@ -8149,7 +8188,7 @@
         <v>15</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>390</v>
+        <v>88</v>
       </c>
       <c r="E235" s="3" t="s">
         <v>388</v>
@@ -8160,19 +8199,19 @@
         <v>15</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>383</v>
+        <v>15</v>
       </c>
       <c r="C236" t="s">
         <v>15</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E236" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="237" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>15</v>
       </c>
@@ -8183,13 +8222,13 @@
         <v>15</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E237" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>15</v>
       </c>
@@ -8200,10 +8239,10 @@
         <v>15</v>
       </c>
       <c r="D238" s="3" t="s">
-        <v>253</v>
+        <v>384</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8217,10 +8256,10 @@
         <v>15</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>549</v>
+        <v>253</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8228,19 +8267,19 @@
         <v>15</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>15</v>
+        <v>383</v>
       </c>
       <c r="C240" t="s">
         <v>15</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E240" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>15</v>
       </c>
@@ -8251,13 +8290,13 @@
         <v>15</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>302</v>
+        <v>548</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="242" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>15</v>
       </c>
@@ -8268,30 +8307,30 @@
         <v>15</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>382</v>
+        <v>302</v>
       </c>
       <c r="E242" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="F242" s="3" t="s">
+    </row>
+    <row r="243" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>15</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C243" t="s">
+        <v>15</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F243" s="3" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>3</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C243" t="s">
-        <v>8</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8299,16 +8338,16 @@
         <v>3</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C244" t="s">
         <v>8</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>256</v>
+        <v>22</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
     </row>
     <row r="245" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8316,33 +8355,33 @@
         <v>3</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C245" t="s">
         <v>8</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>3</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>281</v>
+        <v>230</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
@@ -8350,13 +8389,13 @@
         <v>3</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="C247" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D247" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="E247" s="3" t="s">
         <v>281</v>
@@ -8370,7 +8409,7 @@
         <v>4</v>
       </c>
       <c r="C248" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>23</v>
@@ -8384,13 +8423,13 @@
         <v>3</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C249" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D249" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E249" s="3" t="s">
         <v>281</v>
@@ -8404,7 +8443,7 @@
         <v>5</v>
       </c>
       <c r="C250" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>24</v>
@@ -8413,18 +8452,18 @@
         <v>281</v>
       </c>
     </row>
-    <row r="251" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>3</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C251" t="s">
-        <v>284</v>
+        <v>11</v>
       </c>
       <c r="D251" s="3" t="s">
-        <v>285</v>
+        <v>24</v>
       </c>
       <c r="E251" s="3" t="s">
         <v>281</v>
@@ -8432,16 +8471,16 @@
     </row>
     <row r="252" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
       <c r="C252" t="s">
-        <v>14</v>
+        <v>284</v>
       </c>
       <c r="D252" s="3" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="E252" s="3" t="s">
         <v>281</v>
@@ -8449,16 +8488,16 @@
     </row>
     <row r="253" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C253" t="s">
-        <v>269</v>
+        <v>14</v>
       </c>
       <c r="D253" s="3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E253" s="3" t="s">
         <v>281</v>
@@ -8475,41 +8514,41 @@
         <v>269</v>
       </c>
       <c r="D254" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E254" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="C255" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D255" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E255" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="256" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C256" t="s">
-        <v>14</v>
+        <v>275</v>
       </c>
       <c r="D256" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E256" s="3" t="s">
         <v>281</v>
@@ -8520,19 +8559,16 @@
         <v>45</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="C257" t="s">
         <v>14</v>
       </c>
       <c r="D257" s="3" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="E257" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="F257" s="3" t="s">
-        <v>320</v>
+        <v>281</v>
       </c>
     </row>
     <row r="258" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8546,11 +8582,14 @@
         <v>14</v>
       </c>
       <c r="D258" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E258" s="3" t="s">
         <v>350</v>
       </c>
+      <c r="F258" s="3" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="259" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -8563,7 +8602,7 @@
         <v>14</v>
       </c>
       <c r="D259" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E259" s="3" t="s">
         <v>350</v>
@@ -8580,7 +8619,7 @@
         <v>14</v>
       </c>
       <c r="D260" s="3" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="E260" s="3" t="s">
         <v>350</v>
@@ -8597,7 +8636,7 @@
         <v>14</v>
       </c>
       <c r="D261" s="3" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="E261" s="3" t="s">
         <v>350</v>
@@ -8614,7 +8653,7 @@
         <v>14</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="E262" s="3" t="s">
         <v>350</v>
@@ -8631,7 +8670,7 @@
         <v>14</v>
       </c>
       <c r="D263" s="3" t="s">
-        <v>325</v>
+        <v>351</v>
       </c>
       <c r="E263" s="3" t="s">
         <v>350</v>
@@ -8648,7 +8687,7 @@
         <v>14</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>355</v>
+        <v>325</v>
       </c>
       <c r="E264" s="3" t="s">
         <v>350</v>
@@ -8665,7 +8704,7 @@
         <v>14</v>
       </c>
       <c r="D265" s="3" t="s">
-        <v>327</v>
+        <v>355</v>
       </c>
       <c r="E265" s="3" t="s">
         <v>350</v>
@@ -8682,7 +8721,7 @@
         <v>14</v>
       </c>
       <c r="D266" s="3" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E266" s="3" t="s">
         <v>350</v>
@@ -8699,13 +8738,13 @@
         <v>14</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="E267" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="268" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>45</v>
       </c>
@@ -8716,13 +8755,13 @@
         <v>14</v>
       </c>
       <c r="D268" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E268" s="3" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="269" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>45</v>
       </c>
@@ -8733,13 +8772,10 @@
         <v>14</v>
       </c>
       <c r="D269" s="3" t="s">
-        <v>290</v>
+        <v>356</v>
       </c>
       <c r="E269" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="F269" s="3" t="s">
-        <v>318</v>
+        <v>350</v>
       </c>
     </row>
     <row r="270" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8753,7 +8789,7 @@
         <v>14</v>
       </c>
       <c r="D270" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E270" s="3" t="s">
         <v>340</v>
@@ -8773,10 +8809,10 @@
         <v>14</v>
       </c>
       <c r="D271" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E271" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F271" s="3" t="s">
         <v>318</v>
@@ -8793,7 +8829,7 @@
         <v>14</v>
       </c>
       <c r="D272" s="3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E272" s="3" t="s">
         <v>341</v>
@@ -8813,10 +8849,10 @@
         <v>14</v>
       </c>
       <c r="D273" s="3" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="E273" s="3" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="F273" s="3" t="s">
         <v>318</v>
@@ -8833,7 +8869,7 @@
         <v>14</v>
       </c>
       <c r="D274" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E274" s="3" t="s">
         <v>348</v>
@@ -8842,7 +8878,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="275" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>45</v>
       </c>
@@ -8853,10 +8889,10 @@
         <v>14</v>
       </c>
       <c r="D275" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E275" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F275" s="3" t="s">
         <v>318</v>
@@ -8873,7 +8909,7 @@
         <v>14</v>
       </c>
       <c r="D276" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E276" s="3" t="s">
         <v>349</v>
@@ -8893,7 +8929,7 @@
         <v>14</v>
       </c>
       <c r="D277" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E277" s="3" t="s">
         <v>349</v>
@@ -8913,7 +8949,7 @@
         <v>14</v>
       </c>
       <c r="D278" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E278" s="3" t="s">
         <v>349</v>
@@ -8922,21 +8958,24 @@
         <v>318</v>
       </c>
     </row>
-    <row r="279" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>45</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C279" t="s">
         <v>14</v>
       </c>
       <c r="D279" s="3" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="E279" s="3" t="s">
-        <v>361</v>
+        <v>349</v>
+      </c>
+      <c r="F279" s="3" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="280" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8950,7 +8989,7 @@
         <v>14</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E280" s="3" t="s">
         <v>361</v>
@@ -8967,7 +9006,7 @@
         <v>14</v>
       </c>
       <c r="D281" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E281" s="3" t="s">
         <v>361</v>
@@ -8984,7 +9023,7 @@
         <v>14</v>
       </c>
       <c r="D282" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E282" s="3" t="s">
         <v>361</v>
@@ -9001,13 +9040,13 @@
         <v>14</v>
       </c>
       <c r="D283" s="3" t="s">
-        <v>305</v>
+        <v>360</v>
       </c>
       <c r="E283" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>45</v>
       </c>
@@ -9018,14 +9057,11 @@
         <v>14</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
       <c r="E284" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="F284" s="3" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="285" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
@@ -9038,7 +9074,7 @@
         <v>14</v>
       </c>
       <c r="D285" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E285" s="3" t="s">
         <v>330</v>
@@ -9047,7 +9083,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="286" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>45</v>
       </c>
@@ -9058,7 +9094,7 @@
         <v>14</v>
       </c>
       <c r="D286" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E286" s="3" t="s">
         <v>330</v>
@@ -9078,7 +9114,7 @@
         <v>14</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E287" s="3" t="s">
         <v>330</v>
@@ -9098,7 +9134,7 @@
         <v>14</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E288" s="3" t="s">
         <v>330</v>
@@ -9112,43 +9148,63 @@
         <v>45</v>
       </c>
       <c r="B289" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C289" t="s">
+        <v>14</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E289" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="F289" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>45</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C289" t="s">
-        <v>14</v>
-      </c>
-      <c r="D289" s="3" t="s">
+      <c r="C290" t="s">
+        <v>14</v>
+      </c>
+      <c r="D290" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="E289" s="3" t="s">
+      <c r="E290" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="F289" s="3" t="s">
+      <c r="F290" s="3" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="290" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>45</v>
-      </c>
-      <c r="B290" s="3" t="s">
+    <row r="291" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>45</v>
+      </c>
+      <c r="B291" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C290" t="s">
-        <v>14</v>
-      </c>
-      <c r="D290" s="3" t="s">
+      <c r="C291" t="s">
+        <v>14</v>
+      </c>
+      <c r="D291" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E290" s="3" t="s">
+      <c r="E291" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="F290" s="3" t="s">
+      <c r="F291" s="3" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D291" s="15"/>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D292" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -9709,10 +9765,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9739,224 +9795,224 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43791</v>
+        <v>43819</v>
       </c>
       <c r="B2">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C24" si="0">SUM(B2,-D2)</f>
-        <v>254</v>
+        <f t="shared" ref="C2:C27" si="0">SUM(B2,-D2)</f>
+        <v>255</v>
       </c>
       <c r="D2">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43784</v>
+        <v>43812</v>
       </c>
       <c r="B3">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="D3">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43777</v>
+        <v>43798</v>
       </c>
       <c r="B4">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D4">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43770</v>
+        <v>43791</v>
       </c>
       <c r="B5">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="D5">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>43763</v>
+        <v>43784</v>
       </c>
       <c r="B6">
         <v>284</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>43756</v>
+        <v>43777</v>
       </c>
       <c r="B7">
         <v>284</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D7">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>43749</v>
+        <v>43770</v>
       </c>
       <c r="B8">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D8">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>43742</v>
+        <v>43763</v>
       </c>
       <c r="B9">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="D9">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>43735</v>
+        <v>43756</v>
       </c>
       <c r="B10">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>43728</v>
+        <v>43749</v>
       </c>
       <c r="B11">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="D11">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>43721</v>
+        <v>43742</v>
       </c>
       <c r="B12">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="D12">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>43714</v>
+        <v>43735</v>
       </c>
       <c r="B13">
-        <v>245</v>
+        <v>273</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="D13">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>43707</v>
+        <v>43728</v>
       </c>
       <c r="B14">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>227</v>
       </c>
       <c r="D14">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>43700</v>
+        <v>43721</v>
       </c>
       <c r="B15">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>225</v>
       </c>
       <c r="D15">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>43693</v>
+        <v>43714</v>
       </c>
       <c r="B16">
-        <v>207</v>
+        <v>245</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>204</v>
       </c>
       <c r="D16">
         <v>41</v>
@@ -9964,166 +10020,211 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>43665</v>
+        <v>43707</v>
       </c>
       <c r="B17">
-        <v>199</v>
+        <v>232</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="D17">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <v>43658</v>
+        <v>43700</v>
       </c>
       <c r="B18">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="D18">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>43651</v>
+        <v>43693</v>
       </c>
       <c r="B19">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>166</v>
       </c>
       <c r="D19">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>43644</v>
+        <v>43665</v>
       </c>
       <c r="B20">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D20">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>43638</v>
+        <v>43658</v>
       </c>
       <c r="B21">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="D21">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>43630</v>
+        <v>43651</v>
       </c>
       <c r="B22">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="D22">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>43623</v>
+        <v>43644</v>
       </c>
       <c r="B23">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="D23">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>43616</v>
+        <v>43638</v>
       </c>
       <c r="B24">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="D24">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>43609</v>
+        <v>43630</v>
       </c>
       <c r="B25">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C25">
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>110</v>
       </c>
       <c r="D25">
-        <f>B25-C25</f>
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>43602</v>
+        <v>43623</v>
       </c>
       <c r="B26">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C26">
-        <v>79</v>
+        <f t="shared" si="0"/>
+        <v>102</v>
       </c>
       <c r="D26">
-        <f>B26-C26</f>
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
+        <v>43616</v>
+      </c>
+      <c r="B27">
+        <v>186</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="D27">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14">
+        <v>43609</v>
+      </c>
+      <c r="B28">
+        <v>185</v>
+      </c>
+      <c r="C28">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <f>B28-C28</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>43602</v>
+      </c>
+      <c r="B29">
+        <v>183</v>
+      </c>
+      <c r="C29">
+        <v>79</v>
+      </c>
+      <c r="D29">
+        <f>B29-C29</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
         <v>43595</v>
       </c>
-      <c r="B27">
+      <c r="B30">
         <v>172</v>
       </c>
-      <c r="C27">
+      <c r="C30">
         <v>76</v>
       </c>
-      <c r="D27">
-        <f>B27-C27</f>
+      <c r="D30">
+        <f>B30-C30</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Test Bug Plus test runner scripts (#23)
Test suite "Regression\BugRepro\Bug2259Repro.spec.js" was failing frequently on CircleCI runs due to some odd bug where the Entity Type Drop Down would close automatically shortly after it was opened and before we could select the type we were interested in. I created a complex function that would work around this issue.

Also added a new "RunTests.bat" script and moved the "LoopTests.bat" scrip to the root packages\ui folder.

Also increased the number of LUIS Authoring Keys that were available to test runs.
</commit_message>
<xml_diff>
--- a/packages/ui/cypress/TestGrid.xlsx
+++ b/packages/ui/cypress/TestGrid.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner-UI\cypress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner\packages\ui\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA75BA5-E179-4D86-8D77-3239B14B4732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D5E28C-652E-4CDB-96ED-5F9DC8253AA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -2471,95 +2471,98 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>43826</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43819</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43812</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43798</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2567,12 +2570,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$C$2:$C$30</c:f>
+              <c:f>'Weekly Progress'!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>255</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>255</c:v>
@@ -2581,16 +2584,16 @@
                   <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>254</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>246</c:v>
@@ -2599,63 +2602,66 @@
                   <c:v>246</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>242</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>234</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>229</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>227</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>225</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>204</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>183</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>176</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>166</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>151</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>144</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>132</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>124</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>79</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
@@ -2692,95 +2698,98 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'Weekly Progress'!$A$2:$A$30</c:f>
+              <c:f>'Weekly Progress'!$A$2:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
+                  <c:v>43826</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43819</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43812</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43798</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>43791</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43784</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43777</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43770</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43763</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43756</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>43749</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>43742</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>43735</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43728</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>43721</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>43714</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>43707</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>43700</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>43693</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>43665</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>43658</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>43651</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>43644</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>43638</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>43630</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>43623</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>43616</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>43609</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>43602</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>43595</c:v>
                 </c:pt>
               </c:numCache>
@@ -2788,10 +2797,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Weekly Progress'!$D$2:$D$30</c:f>
+              <c:f>'Weekly Progress'!$D$2:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
@@ -2802,16 +2811,16 @@
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>33</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>38</c:v>
@@ -2820,63 +2829,66 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>34</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>93</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="28">
                   <c:v>104</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="29">
                   <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
@@ -3648,13 +3660,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3716,8 +3728,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D30" totalsRowShown="0">
-  <autoFilter ref="A1:D30" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2150B3DF-BB2E-4B60-8D55-F742950E367A}" name="Table15" displayName="Table15" ref="A1:D31" totalsRowShown="0">
+  <autoFilter ref="A1:D31" xr:uid="{186D535B-B5B9-4A39-B07E-81AB77ACC099}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5585221-FAE2-4C1B-938F-A848BA5771FE}" name="Column1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{6229C132-74E5-42FB-A81D-37498D4788E1}" name="Scenarios"/>
@@ -4123,7 +4135,7 @@
   <dimension ref="A1:F292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
@@ -9765,9 +9777,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDA4FAC-EB22-4F76-B22F-D4B2A8D49793}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C3" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
@@ -9795,14 +9807,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
-        <v>43819</v>
+        <v>43826</v>
       </c>
       <c r="B2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C27" si="0">SUM(B2,-D2)</f>
-        <v>255</v>
+        <f t="shared" ref="C2:C28" si="0">SUM(B2,-D2)</f>
+        <v>256</v>
       </c>
       <c r="D2">
         <v>35</v>
@@ -9810,7 +9822,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>43812</v>
+        <v>43819</v>
       </c>
       <c r="B3">
         <v>290</v>
@@ -9825,7 +9837,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>43798</v>
+        <v>43812</v>
       </c>
       <c r="B4">
         <v>290</v>
@@ -9840,67 +9852,67 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>43791</v>
+        <v>43798</v>
       </c>
       <c r="B5">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D5">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>43784</v>
+        <v>43791</v>
       </c>
       <c r="B6">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="D6">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>43777</v>
+        <v>43784</v>
       </c>
       <c r="B7">
         <v>284</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D7">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>43770</v>
+        <v>43777</v>
       </c>
       <c r="B8">
         <v>284</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D8">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>43763</v>
+        <v>43770</v>
       </c>
       <c r="B9">
         <v>284</v>
@@ -9915,7 +9927,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>43756</v>
+        <v>43763</v>
       </c>
       <c r="B10">
         <v>284</v>
@@ -9930,29 +9942,29 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>43749</v>
+        <v>43756</v>
       </c>
       <c r="B11">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D11">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>43742</v>
+        <v>43749</v>
       </c>
       <c r="B12">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="D12">
         <v>41</v>
@@ -9960,104 +9972,104 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>43735</v>
+        <v>43742</v>
       </c>
       <c r="B13">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="D13">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>43728</v>
+        <v>43735</v>
       </c>
       <c r="B14">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D14">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>43721</v>
+        <v>43728</v>
       </c>
       <c r="B15">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D15">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>43714</v>
+        <v>43721</v>
       </c>
       <c r="B16">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="D16">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>43707</v>
+        <v>43714</v>
       </c>
       <c r="B17">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="D17">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
-        <v>43700</v>
+        <v>43707</v>
       </c>
       <c r="B18">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D18">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
-        <v>43693</v>
+        <v>43700</v>
       </c>
       <c r="B19">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D19">
         <v>41</v>
@@ -10065,44 +10077,44 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
-        <v>43665</v>
+        <v>43693</v>
       </c>
       <c r="B20">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="D20">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
-        <v>43658</v>
+        <v>43665</v>
       </c>
       <c r="B21">
         <v>199</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D21">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
-        <v>43651</v>
+        <v>43658</v>
       </c>
       <c r="B22">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D22">
         <v>54</v>
@@ -10110,121 +10122,136 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
-        <v>43644</v>
+        <v>43651</v>
       </c>
       <c r="B23">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="D23">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
-        <v>43638</v>
+        <v>43644</v>
       </c>
       <c r="B24">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="D24">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>43630</v>
+        <v>43638</v>
       </c>
       <c r="B25">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="D25">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
-        <v>43623</v>
+        <v>43630</v>
       </c>
       <c r="B26">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D26">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
-        <v>43616</v>
+        <v>43623</v>
       </c>
       <c r="B27">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D27">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
-        <v>43609</v>
+        <v>43616</v>
       </c>
       <c r="B28">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C28">
-        <v>83</v>
+        <f t="shared" si="0"/>
+        <v>93</v>
       </c>
       <c r="D28">
-        <f>B28-C28</f>
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
-        <v>43602</v>
+        <v>43609</v>
       </c>
       <c r="B29">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C29">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D29">
         <f>B29-C29</f>
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
-        <v>43595</v>
+        <v>43602</v>
       </c>
       <c r="B30">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="C30">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D30">
         <f>B30-C30</f>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
+        <v>43595</v>
+      </c>
+      <c r="B31">
+        <v>172</v>
+      </c>
+      <c r="C31">
+        <v>76</v>
+      </c>
+      <c r="D31">
+        <f>B31-C31</f>
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: moving this test from Tools into our Regression tests
</commit_message>
<xml_diff>
--- a/packages/ui/cypress/TestGrid.xlsx
+++ b/packages/ui/cypress/TestGrid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner\packages\ui\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5DA776-2E10-44B9-BF32-F11053890560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9596633-F830-417E-9BD8-D6401FE8805F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -1291,9 +1291,6 @@
     <t>Verify that "Train Dialog" filter button navigates to Train Dialog pane and shows only the Train Dialogs in the list that use the selected Action.</t>
   </si>
   <si>
-    <t>Tools/EntityActionMissingUserTurn</t>
-  </si>
-  <si>
     <t>Start with a model with 2 Train Dialogs that could be merged - Edit Train Dialog with a single turn involving 1 Entity label and a Bot Response that renders that Entity - Add a simple text User turn - Score a simple Text Action - Delete the User turn that was just added - Save TD as is. (Bug 2191)</t>
   </si>
   <si>
@@ -2191,6 +2188,9 @@
   </si>
   <si>
     <t>Edit an Action that has "Prompt on unexpected…" checked and a Disqualifying Condition - remove a Disqualifying Condition - Save - Verify that it saved without error (Bug 2379)</t>
+  </si>
+  <si>
+    <t>BugRepro/Bug2191Repro</t>
   </si>
 </sst>
 </file>
@@ -4145,7 +4145,7 @@
         <v>256</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -4159,8 +4159,8 @@
   <dimension ref="A1:F295"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E237" sqref="E237"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4462,7 +4462,7 @@
         <v>190</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4479,7 +4479,7 @@
         <v>191</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4493,10 +4493,10 @@
         <v>25</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4513,7 +4513,7 @@
         <v>192</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4530,7 +4530,7 @@
         <v>365</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4547,7 +4547,7 @@
         <v>194</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4564,7 +4564,7 @@
         <v>363</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4581,7 +4581,7 @@
         <v>364</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4598,7 +4598,7 @@
         <v>360</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4615,7 +4615,7 @@
         <v>362</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -4720,10 +4720,10 @@
         <v>26</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4737,10 +4737,10 @@
         <v>26</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4757,7 +4757,7 @@
         <v>367</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4765,16 +4765,16 @@
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E34" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4782,16 +4782,16 @@
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C35" t="s">
         <v>26</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E35" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4808,7 +4808,7 @@
         <v>196</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
         <v>366</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>26</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>371</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4859,7 +4859,7 @@
         <v>197</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -4876,7 +4876,7 @@
         <v>208</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4901,16 +4901,16 @@
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="C42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>469</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4927,7 +4927,7 @@
         <v>215</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>216</v>
@@ -4947,7 +4947,7 @@
         <v>209</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
@@ -4961,10 +4961,10 @@
         <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>217</v>
@@ -4981,13 +4981,13 @@
         <v>17</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -5004,7 +5004,7 @@
         <v>93</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -5021,7 +5021,7 @@
         <v>178</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,7 +5038,7 @@
         <v>179</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -5055,7 +5055,7 @@
         <v>182</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5072,7 +5072,7 @@
         <v>183</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>86</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5123,7 +5123,7 @@
         <v>220</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5140,7 +5140,7 @@
         <v>221</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
         <v>98</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5242,7 +5242,7 @@
         <v>32</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5259,7 +5259,7 @@
         <v>33</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5293,7 +5293,7 @@
         <v>87</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5301,13 +5301,13 @@
         <v>28</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C65" t="s">
         <v>26</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>274</v>
@@ -5318,13 +5318,13 @@
         <v>28</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C66" t="s">
         <v>26</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>274</v>
@@ -5341,10 +5341,10 @@
         <v>14</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5358,10 +5358,10 @@
         <v>14</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5378,7 +5378,7 @@
         <v>300</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5395,7 +5395,7 @@
         <v>301</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5412,7 +5412,7 @@
         <v>302</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5429,7 +5429,7 @@
         <v>303</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5446,7 +5446,7 @@
         <v>304</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>299</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5477,10 +5477,10 @@
         <v>14</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -5494,10 +5494,10 @@
         <v>14</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -5511,10 +5511,10 @@
         <v>14</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5528,10 +5528,10 @@
         <v>14</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5545,10 +5545,10 @@
         <v>14</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -5562,10 +5562,10 @@
         <v>14</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5579,10 +5579,10 @@
         <v>14</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -5596,10 +5596,10 @@
         <v>14</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5613,10 +5613,10 @@
         <v>14</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -5630,10 +5630,10 @@
         <v>14</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -5647,10 +5647,10 @@
         <v>14</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -5664,10 +5664,10 @@
         <v>14</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5681,10 +5681,10 @@
         <v>14</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -5698,10 +5698,10 @@
         <v>14</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5715,10 +5715,10 @@
         <v>14</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5732,10 +5732,10 @@
         <v>14</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -5766,10 +5766,10 @@
         <v>14</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -5783,10 +5783,10 @@
         <v>14</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -5800,10 +5800,10 @@
         <v>14</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5817,10 +5817,10 @@
         <v>14</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -5834,10 +5834,10 @@
         <v>14</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -5851,10 +5851,10 @@
         <v>14</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -5868,10 +5868,10 @@
         <v>14</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -5885,10 +5885,10 @@
         <v>14</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5902,10 +5902,10 @@
         <v>14</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5919,10 +5919,10 @@
         <v>14</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5936,10 +5936,10 @@
         <v>14</v>
       </c>
       <c r="D102" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E102" s="3" t="s">
         <v>449</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5953,10 +5953,10 @@
         <v>14</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -5964,16 +5964,16 @@
         <v>45</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C104" t="s">
+        <v>14</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="C104" t="s">
-        <v>14</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>409</v>
-      </c>
       <c r="E104" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -5981,16 +5981,16 @@
         <v>45</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C105" t="s">
         <v>14</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5998,16 +5998,16 @@
         <v>45</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6015,16 +6015,16 @@
         <v>45</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C107" t="s">
+        <v>14</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="C107" t="s">
-        <v>14</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>413</v>
-      </c>
       <c r="E107" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6032,16 +6032,16 @@
         <v>45</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C108" t="s">
         <v>14</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6049,16 +6049,16 @@
         <v>45</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C109" t="s">
         <v>14</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -6160,7 +6160,7 @@
         <v>62</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -6185,16 +6185,16 @@
         <v>45</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C117" t="s">
         <v>14</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6208,10 +6208,10 @@
         <v>14</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6219,16 +6219,16 @@
         <v>45</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C119" t="s">
         <v>14</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6236,16 +6236,16 @@
         <v>45</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C120" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -6253,16 +6253,16 @@
         <v>45</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -6270,16 +6270,16 @@
         <v>45</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C122" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="C122" t="s">
-        <v>14</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>552</v>
-      </c>
       <c r="E122" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -6287,16 +6287,16 @@
         <v>45</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6304,16 +6304,16 @@
         <v>45</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C124" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6321,16 +6321,16 @@
         <v>45</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C125" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -6338,16 +6338,16 @@
         <v>45</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C126" t="s">
         <v>14</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -6355,16 +6355,16 @@
         <v>45</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C127" t="s">
         <v>14</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -6378,10 +6378,10 @@
         <v>14</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>368</v>
+        <v>560</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6395,10 +6395,10 @@
         <v>14</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6412,10 +6412,10 @@
         <v>14</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6429,10 +6429,10 @@
         <v>14</v>
       </c>
       <c r="D131" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E131" s="3" t="s">
         <v>433</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -6446,10 +6446,10 @@
         <v>14</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6463,10 +6463,10 @@
         <v>14</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6480,10 +6480,10 @@
         <v>14</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6497,10 +6497,10 @@
         <v>14</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6514,10 +6514,10 @@
         <v>14</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>307</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -6551,7 +6551,7 @@
         <v>306</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6565,10 +6565,10 @@
         <v>14</v>
       </c>
       <c r="D139" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>436</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6576,16 +6576,16 @@
         <v>45</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C140" t="s">
         <v>14</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6593,16 +6593,16 @@
         <v>45</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C141" t="s">
         <v>14</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6610,16 +6610,16 @@
         <v>45</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C142" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6627,16 +6627,16 @@
         <v>45</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C143" t="s">
         <v>14</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -6644,16 +6644,16 @@
         <v>45</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C144" t="s">
         <v>14</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6661,16 +6661,16 @@
         <v>45</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C145" t="s">
         <v>14</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -6911,7 +6911,7 @@
         <v>63</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -6962,7 +6962,7 @@
         <v>280</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -6976,10 +6976,10 @@
         <v>14</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -6993,10 +6993,10 @@
         <v>14</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7010,10 +7010,10 @@
         <v>14</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7027,10 +7027,10 @@
         <v>14</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -7044,10 +7044,10 @@
         <v>14</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7061,10 +7061,10 @@
         <v>14</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -7078,10 +7078,10 @@
         <v>12</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7089,16 +7089,16 @@
         <v>45</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C170" t="s">
         <v>14</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7106,16 +7106,16 @@
         <v>45</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C171" t="s">
         <v>14</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7123,19 +7123,19 @@
         <v>45</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="C172" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="C172" t="s">
-        <v>14</v>
-      </c>
-      <c r="D172" s="8" t="s">
+      <c r="E172" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="F172" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="F172" s="3" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7149,10 +7149,10 @@
         <v>14</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7160,16 +7160,16 @@
         <v>45</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C174" t="s">
         <v>12</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7186,7 +7186,7 @@
         <v>279</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7200,10 +7200,10 @@
         <v>14</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7217,10 +7217,10 @@
         <v>14</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7234,10 +7234,10 @@
         <v>14</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7251,10 +7251,10 @@
         <v>14</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -7268,10 +7268,10 @@
         <v>14</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="181" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7285,10 +7285,10 @@
         <v>14</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7302,10 +7302,10 @@
         <v>14</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -7319,10 +7319,10 @@
         <v>14</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E183" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -7336,10 +7336,10 @@
         <v>14</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7353,10 +7353,10 @@
         <v>14</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E185" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="186" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7370,10 +7370,10 @@
         <v>14</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7387,10 +7387,10 @@
         <v>14</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7404,10 +7404,10 @@
         <v>14</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7421,10 +7421,10 @@
         <v>14</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7438,10 +7438,10 @@
         <v>14</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E190" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7455,10 +7455,10 @@
         <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E191" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7472,10 +7472,10 @@
         <v>14</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F192" s="3" t="s">
         <v>297</v>
@@ -7492,10 +7492,10 @@
         <v>14</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E193" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="194" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -7509,10 +7509,10 @@
         <v>14</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="195" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -7526,10 +7526,10 @@
         <v>14</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E195" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="196" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -7764,10 +7764,10 @@
         <v>14</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F209" s="3" t="s">
         <v>293</v>
@@ -7784,10 +7784,10 @@
         <v>14</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E210" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="211" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7801,10 +7801,10 @@
         <v>14</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E211" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="212" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7818,10 +7818,10 @@
         <v>14</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E212" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="213" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -7835,10 +7835,10 @@
         <v>14</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="214" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -7852,10 +7852,10 @@
         <v>14</v>
       </c>
       <c r="D214" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="E214" s="3" t="s">
         <v>458</v>
-      </c>
-      <c r="E214" s="3" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -7869,7 +7869,7 @@
         <v>14</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E215" s="3" t="s">
         <v>274</v>
@@ -7906,7 +7906,7 @@
         <v>14</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E217" s="3" t="s">
         <v>274</v>
@@ -7926,7 +7926,7 @@
         <v>14</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E218" s="3" t="s">
         <v>274</v>
@@ -7946,7 +7946,7 @@
         <v>14</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E219" s="3" t="s">
         <v>274</v>
@@ -7966,10 +7966,10 @@
         <v>14</v>
       </c>
       <c r="D220" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="E220" s="3" t="s">
         <v>500</v>
-      </c>
-      <c r="E220" s="3" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="221" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8051,10 +8051,10 @@
         <v>14</v>
       </c>
       <c r="D225" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="E225" s="3" t="s">
         <v>505</v>
-      </c>
-      <c r="E225" s="3" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="226" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8173,10 +8173,10 @@
         <v>312</v>
       </c>
       <c r="E232" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="F232" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="F232" s="3" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8201,16 +8201,16 @@
         <v>45</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C234" t="s">
         <v>14</v>
       </c>
       <c r="D234" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="235" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8218,16 +8218,16 @@
         <v>45</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C235" t="s">
         <v>14</v>
       </c>
       <c r="D235" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="E235" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="236" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8235,16 +8235,16 @@
         <v>45</v>
       </c>
       <c r="B236" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C236" t="s">
+        <v>14</v>
+      </c>
+      <c r="D236" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="C236" t="s">
-        <v>14</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>510</v>
-      </c>
       <c r="E236" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="237" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -8261,7 +8261,7 @@
         <v>89</v>
       </c>
       <c r="E237" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
@@ -8278,7 +8278,7 @@
         <v>88</v>
       </c>
       <c r="E238" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="239" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8292,10 +8292,10 @@
         <v>15</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E239" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="240" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8303,16 +8303,16 @@
         <v>15</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C240" t="s">
         <v>15</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E240" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="241" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8320,16 +8320,16 @@
         <v>15</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C241" t="s">
         <v>15</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E241" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="242" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8337,7 +8337,7 @@
         <v>15</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C242" t="s">
         <v>15</v>
@@ -8346,7 +8346,7 @@
         <v>247</v>
       </c>
       <c r="E242" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="243" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8354,16 +8354,16 @@
         <v>15</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C243" t="s">
         <v>15</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E243" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="244" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8377,10 +8377,10 @@
         <v>15</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
@@ -8397,7 +8397,7 @@
         <v>295</v>
       </c>
       <c r="E245" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="246" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -8411,10 +8411,10 @@
         <v>15</v>
       </c>
       <c r="D246" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E246" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F246" s="3" t="s">
         <v>296</v>
@@ -8434,7 +8434,7 @@
         <v>22</v>
       </c>
       <c r="E247" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -8468,7 +8468,7 @@
         <v>64</v>
       </c>
       <c r="E249" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.25">
@@ -9281,13 +9281,13 @@
         <v>14</v>
       </c>
       <c r="D294" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="F294" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="E294" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="F294" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: completed review of support components
</commit_message>
<xml_diff>
--- a/packages/ui/cypress/TestGrid.xlsx
+++ b/packages/ui/cypress/TestGrid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ConversationLearner\packages\ui\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C274724-6D0A-4B52-82ED-D005624A8530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177595A1-4068-479A-A052-EA5B4094A94C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E372DEC-327E-4746-A167-3846B8704516}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1699" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="595">
   <si>
     <t>Page</t>
   </si>
@@ -2293,6 +2293,9 @@
   </si>
   <si>
     <t>We only have a few branching tests. There must be more scenarios that we can cover around this feature. Search for "BranchChatTurn" to see what is currently covered.</t>
+  </si>
+  <si>
+    <t>API callback throws an exception - Verify only one chat message shows up (as opposed to the 2 that show up with bug 2441)</t>
   </si>
 </sst>
 </file>
@@ -3840,8 +3843,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F319" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A1:F319" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3D8D34B5-BAEA-4C8B-8DF5-C01D86E62957}" name="Table1" displayName="Table1" ref="A1:F320" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A1:F320" xr:uid="{B5F7D8EE-9D8F-47A2-A197-9D8037549501}"/>
   <tableColumns count="6">
     <tableColumn id="4" xr3:uid="{7905D971-B220-4A95-B9FD-7D1376A44B1E}" name="Area"/>
     <tableColumn id="5" xr3:uid="{52A5D5B9-9F85-46B1-A753-74A933A948A7}" name="Feature" dataDxfId="6"/>
@@ -4274,11 +4277,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFC66FE2-0B4E-44F5-88F5-E30061E2A753}">
-  <dimension ref="A1:F300"/>
+  <dimension ref="A1:F301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E300" sqref="E300"/>
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E287" sqref="E287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9303,21 +9306,21 @@
         <v>302</v>
       </c>
     </row>
-    <row r="287" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>44</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C287" t="s">
         <v>14</v>
       </c>
       <c r="D287" s="3" t="s">
-        <v>341</v>
+        <v>594</v>
       </c>
       <c r="E287" s="3" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="288" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9331,7 +9334,7 @@
         <v>14</v>
       </c>
       <c r="D288" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E288" s="3" t="s">
         <v>345</v>
@@ -9348,7 +9351,7 @@
         <v>14</v>
       </c>
       <c r="D289" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E289" s="3" t="s">
         <v>345</v>
@@ -9365,7 +9368,7 @@
         <v>14</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E290" s="3" t="s">
         <v>345</v>
@@ -9382,13 +9385,13 @@
         <v>14</v>
       </c>
       <c r="D291" s="3" t="s">
-        <v>290</v>
+        <v>344</v>
       </c>
       <c r="E291" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>44</v>
       </c>
@@ -9399,14 +9402,11 @@
         <v>14</v>
       </c>
       <c r="D292" s="3" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
       <c r="E292" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F292" s="3" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="293" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
@@ -9419,7 +9419,7 @@
         <v>14</v>
       </c>
       <c r="D293" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E293" s="3" t="s">
         <v>314</v>
@@ -9428,7 +9428,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="294" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>44</v>
       </c>
@@ -9439,7 +9439,7 @@
         <v>14</v>
       </c>
       <c r="D294" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E294" s="3" t="s">
         <v>314</v>
@@ -9459,7 +9459,7 @@
         <v>14</v>
       </c>
       <c r="D295" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E295" s="3" t="s">
         <v>314</v>
@@ -9479,7 +9479,7 @@
         <v>14</v>
       </c>
       <c r="D296" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E296" s="3" t="s">
         <v>314</v>
@@ -9493,60 +9493,80 @@
         <v>44</v>
       </c>
       <c r="B297" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C297" t="s">
+        <v>14</v>
+      </c>
+      <c r="D297" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E297" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F297" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>44</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C297" t="s">
-        <v>14</v>
-      </c>
-      <c r="D297" s="3" t="s">
+      <c r="C298" t="s">
+        <v>14</v>
+      </c>
+      <c r="D298" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="E297" s="3" t="s">
+      <c r="E298" s="3" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="298" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>44</v>
-      </c>
-      <c r="B298" s="3" t="s">
+    <row r="299" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>44</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C298" t="s">
-        <v>14</v>
-      </c>
-      <c r="D298" s="3" t="s">
+      <c r="C299" t="s">
+        <v>14</v>
+      </c>
+      <c r="D299" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E298" s="3" t="s">
+      <c r="E299" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="F298" s="3" t="s">
+      <c r="F299" s="3" t="s">
         <v>377</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>591</v>
-      </c>
-      <c r="D299" s="15" t="s">
-        <v>592</v>
-      </c>
-      <c r="E299" s="3" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="300" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>591</v>
       </c>
-      <c r="B300" s="3" t="s">
+      <c r="D300" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>591</v>
+      </c>
+      <c r="B301" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D300" s="15" t="s">
+      <c r="D301" s="15" t="s">
         <v>593</v>
       </c>
-      <c r="E300" s="3" t="s">
+      <c r="E301" s="3" t="s">
         <v>561</v>
       </c>
     </row>

</xml_diff>